<commit_message>
migration of the site to make it scalable
</commit_message>
<xml_diff>
--- a/static/campionato/squadre/vispesaro/molina/molina.xlsx
+++ b/static/campionato/squadre/vispesaro/molina/molina.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reus3111/Clip_Pianese/sito_web/campionato/squadre/vispesaro/molina/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reus3111/Clip_Campobasso/sito_web/campionato/squadre/vispesaro/molina/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FA5EE1-D6CE-074F-AA8C-99C2DE639ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B482A1-F4CE-554B-BB31-5832F630C9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Partita</t>
   </si>
@@ -86,13 +86,22 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=aClOLiFuTB0&amp;list=PLD64-55Vi5w75GRKJZRxuA33GOm4IaLDb&amp;index=3&amp;pp=gAQBiAQB</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=yIB87ew2T5E&amp;list=PLD64-55Vi5w75GRKJZRxuA33GOm4IaLDb&amp;index=1</t>
+  </si>
+  <si>
+    <t>Vis Pesaro-Lucchese</t>
+  </si>
+  <si>
+    <t>0-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +113,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,16 +158,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,13 +479,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="91.1640625" customWidth="1"/>
+    <col min="6" max="9" width="20.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -490,56 +521,56 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2">
-        <v>9</v>
-      </c>
-      <c r="G2">
-        <v>28</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="2">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2">
+        <v>21</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3">
-        <v>29.5</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
         <v>17</v>
@@ -550,25 +581,25 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G4">
-        <v>7</v>
+        <v>29.5</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
@@ -577,7 +608,39 @@
         <v>18</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{8AA7F520-80AB-904C-B08A-08214AC5C722}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>